<commit_message>
now indexes model fit for correct coefficients, adds a script to check those coefficients explicitly
</commit_message>
<xml_diff>
--- a/excel_calculators/Combined_Calculator.xlsx
+++ b/excel_calculators/Combined_Calculator.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Temp_C (°C)</t>
   </si>
@@ -21,6 +21,12 @@
   </si>
   <si>
     <t xml:space="preserve">Pred_pCO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">log10(pCO2) = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1.482088436399 +  1.302620509340*Z7 +  0.038254786156*T7 +  -0.139692743505*Z7^2 +  -0.037555238467*Z7*T7 +  -0.000769389499*T7^2 +  0.019624637219*Z7^2*T7 +  0.001235261007*Z7*T7^2 +  -0.000657950594*Z7^2*T7^2)</t>
   </si>
 </sst>
 </file>
@@ -359,9 +365,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="20" max="20" width="12.71" hidden="0" customWidth="1"/>
-    <col min="26" max="26" width="4.71" hidden="0" customWidth="1"/>
-    <col min="30" max="30" width="9.71" hidden="0" customWidth="1"/>
+    <col min="20" max="20" width="15.71" hidden="0" customWidth="1"/>
+    <col min="26" max="26" width="15.71" hidden="0" customWidth="1"/>
+    <col min="30" max="30" width="15.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6">
@@ -383,7 +389,15 @@
         <v>0.85</v>
       </c>
       <c r="AD7" t="str">
-        <f>=10^(1.7804+0.7498*Z7+-0.0026*T7+0.1412*Z7^2+0.0457*Z7*T7+4e-04*T7^2+-0.0239*Z7^2*T7+-0.0012*Z7*T7^2+0.00065*Z7^2*T7^2)</f>
+        <f>=10^(1.482088436399 + 1.302620509340*Z7 + 0.038254786156*T7 + -0.139692743505*Z7^2 + -0.037555238467*Z7*T7 + -0.000769389499*T7^2 + 0.019624637219*Z7^2*T7 + 0.001235261007*Z7*T7^2 + -0.000657950594*Z7^2*T7^2)</f>
+      </c>
+    </row>
+    <row r="9">
+      <c r="T9" t="s">
+        <v>3</v>
+      </c>
+      <c r="U9" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>